<commit_message>
Examples added for Aspose.Cells for .NET 18.11.0
</commit_message>
<xml_diff>
--- a/Examples/Data/01_SourceDirectory/sampleDataValidationRules.xlsx
+++ b/Examples/Data/01_SourceDirectory/sampleDataValidationRules.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16729"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Download\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AsposeProjects\GitRepo\Net\Aspose_Cells_for_NET\Examples\Data\01_SourceDirectory\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B1FFBAB7-1FB9-4E15-88D0-105ACCEC8193}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,12 +19,8 @@
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -77,7 +74,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -412,27 +409,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="C1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2">
+  <dataValidations count="3">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>20</formula1>
       <formula2>30</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>10</formula1>
       <formula2>20</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1" xr:uid="{32CED5D8-962A-4FEE-9420-C3471B776CD9}">
+      <formula1>1</formula1>
+      <formula2>999999999999</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>